<commit_message>
fixed WRR for not dynamic weights
</commit_message>
<xml_diff>
--- a/results/configuration_2/experiment_results.xlsx
+++ b/results/configuration_2/experiment_results.xlsx
@@ -613,19 +613,19 @@
         <v>1</v>
       </c>
       <c r="P4" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="Q4" t="n">
-        <v>2.8</v>
+        <v>4.9</v>
       </c>
       <c r="R4" t="n">
-        <v>14</v>
+        <v>24.5</v>
       </c>
       <c r="S4" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="T4" t="n">
-        <v>1680</v>
+        <v>2940</v>
       </c>
       <c r="V4" t="n">
         <v>1</v>
@@ -687,19 +687,19 @@
         <v>2</v>
       </c>
       <c r="P5" t="n">
-        <v>64</v>
+        <v>49.5</v>
       </c>
       <c r="Q5" t="n">
-        <v>2.8</v>
+        <v>4.8</v>
       </c>
       <c r="R5" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="S5" t="n">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="T5" t="n">
-        <v>1680</v>
+        <v>2880</v>
       </c>
       <c r="V5" t="n">
         <v>2</v>
@@ -761,19 +761,19 @@
         <v>3</v>
       </c>
       <c r="P6" t="n">
-        <v>64</v>
+        <v>47.5</v>
       </c>
       <c r="Q6" t="n">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="R6" t="n">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="S6" t="n">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="T6" t="n">
-        <v>1680</v>
+        <v>1140</v>
       </c>
       <c r="V6" t="n">
         <v>3</v>
@@ -835,19 +835,19 @@
         <v>4</v>
       </c>
       <c r="P7" t="n">
-        <v>64</v>
+        <v>47.5</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.8</v>
+        <v>1.9</v>
       </c>
       <c r="R7" t="n">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="S7" t="n">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="T7" t="n">
-        <v>1680</v>
+        <v>1140</v>
       </c>
       <c r="V7" t="n">
         <v>4</v>
@@ -909,19 +909,19 @@
         <v>5</v>
       </c>
       <c r="P8" t="n">
-        <v>40.9836</v>
+        <v>47.1311</v>
       </c>
       <c r="Q8" t="n">
-        <v>2.6</v>
+        <v>1.4</v>
       </c>
       <c r="R8" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S8" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="T8" t="n">
-        <v>1560</v>
+        <v>840</v>
       </c>
       <c r="V8" t="n">
         <v>5</v>
@@ -983,19 +983,19 @@
         <v>6</v>
       </c>
       <c r="P9" t="n">
-        <v>40.9836</v>
+        <v>45.9016</v>
       </c>
       <c r="Q9" t="n">
-        <v>2.6</v>
+        <v>0.8</v>
       </c>
       <c r="R9" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="S9" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="T9" t="n">
-        <v>1560</v>
+        <v>480</v>
       </c>
       <c r="V9" t="n">
         <v>6</v>
@@ -1057,19 +1057,19 @@
         <v>7</v>
       </c>
       <c r="P10" t="n">
-        <v>40.9836</v>
+        <v>33.1967</v>
       </c>
       <c r="Q10" t="n">
-        <v>2.6</v>
+        <v>3.15</v>
       </c>
       <c r="R10" t="n">
-        <v>13</v>
+        <v>15.75</v>
       </c>
       <c r="S10" t="n">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="T10" t="n">
-        <v>1560</v>
+        <v>1890</v>
       </c>
       <c r="V10" t="n">
         <v>7</v>
@@ -1131,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="P11" t="n">
-        <v>40.9836</v>
+        <v>44.0574</v>
       </c>
       <c r="Q11" t="n">
         <v>2.6</v>
@@ -1140,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="S11" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="T11" t="n">
         <v>1560</v>
@@ -1205,19 +1205,19 @@
         <v>9</v>
       </c>
       <c r="P12" t="n">
-        <v>40.9836</v>
+        <v>47.541</v>
       </c>
       <c r="Q12" t="n">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="R12" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="S12" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="T12" t="n">
-        <v>1560</v>
+        <v>960</v>
       </c>
       <c r="V12" t="n">
         <v>9</v>
@@ -1279,19 +1279,19 @@
         <v>10</v>
       </c>
       <c r="P13" t="n">
-        <v>40.9836</v>
+        <v>46.3115</v>
       </c>
       <c r="Q13" t="n">
-        <v>2.6</v>
+        <v>1.9</v>
       </c>
       <c r="R13" t="n">
-        <v>13</v>
+        <v>9.5</v>
       </c>
       <c r="S13" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="T13" t="n">
-        <v>1560</v>
+        <v>1140</v>
       </c>
       <c r="V13" t="n">
         <v>10</v>
@@ -1353,19 +1353,19 @@
         <v>11</v>
       </c>
       <c r="P14" t="n">
-        <v>40.9836</v>
+        <v>47.541</v>
       </c>
       <c r="Q14" t="n">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="R14" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="S14" t="n">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="T14" t="n">
-        <v>1560</v>
+        <v>960</v>
       </c>
       <c r="V14" t="n">
         <v>11</v>
@@ -1427,19 +1427,19 @@
         <v>12</v>
       </c>
       <c r="P15" t="n">
-        <v>22.7273</v>
+        <v>37.3864</v>
       </c>
       <c r="Q15" t="n">
-        <v>2.6</v>
+        <v>5.45</v>
       </c>
       <c r="R15" t="n">
-        <v>13</v>
+        <v>27.25</v>
       </c>
       <c r="S15" t="n">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="T15" t="n">
-        <v>1560</v>
+        <v>3270</v>
       </c>
       <c r="V15" t="n">
         <v>12</v>

</xml_diff>